<commit_message>
Hotfix - corrigido bugs que não identificava o produto corretamente.
</commit_message>
<xml_diff>
--- a/arquivos/fonte_de_dados.xlsx
+++ b/arquivos/fonte_de_dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Documents\GitHub\InventariadorJohnmar\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87C152F-4A8A-4945-A4C8-9E286F819449}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72879D8-E7D0-4441-A68F-BFB67F770B55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20760" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9448,7 +9448,7 @@
   <dimension ref="A1:G1252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9521,7 +9521,7 @@
         <v>17898954589036</v>
       </c>
       <c r="E3" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -9544,7 +9544,7 @@
         <v>17898953272199</v>
       </c>
       <c r="E4" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -9567,7 +9567,7 @@
         <v>17896509926961</v>
       </c>
       <c r="E5" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -9590,7 +9590,7 @@
         <v>17896509926923</v>
       </c>
       <c r="E6" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
@@ -9613,7 +9613,7 @@
         <v>17896509905133</v>
       </c>
       <c r="E7" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -9636,7 +9636,7 @@
         <v>37896509905168</v>
       </c>
       <c r="E8" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
@@ -9659,7 +9659,7 @@
         <v>37896509905175</v>
       </c>
       <c r="E9" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
@@ -9682,7 +9682,7 @@
         <v>17896509905157</v>
       </c>
       <c r="E10" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
         <v>18</v>
@@ -9705,7 +9705,7 @@
         <v>37896509905601</v>
       </c>
       <c r="E11" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
@@ -9728,7 +9728,7 @@
         <v>17898924640071</v>
       </c>
       <c r="E12" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
         <v>32</v>
@@ -9751,7 +9751,7 @@
         <v>17898947389544</v>
       </c>
       <c r="E13" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
         <v>35</v>
@@ -9774,7 +9774,7 @@
         <v>17898947390281</v>
       </c>
       <c r="E14" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
         <v>32</v>
@@ -9797,7 +9797,7 @@
         <v>17898924640095</v>
       </c>
       <c r="E15" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
         <v>40</v>
@@ -9820,7 +9820,7 @@
         <v>17898954589562</v>
       </c>
       <c r="E16" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
         <v>43</v>
@@ -9843,7 +9843,7 @@
         <v>17898924640101</v>
       </c>
       <c r="E17" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
         <v>46</v>
@@ -9866,7 +9866,7 @@
         <v>17898924640958</v>
       </c>
       <c r="E18" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
         <v>35</v>
@@ -9889,7 +9889,7 @@
         <v>17898947389551</v>
       </c>
       <c r="E19" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
         <v>51</v>
@@ -9912,7 +9912,7 @@
         <v>17898954589715</v>
       </c>
       <c r="E20" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
         <v>54</v>
@@ -9935,7 +9935,7 @@
         <v>17898954589708</v>
       </c>
       <c r="E21" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
         <v>57</v>
@@ -9958,7 +9958,7 @@
         <v>17898924640057</v>
       </c>
       <c r="E22" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
         <v>51</v>
@@ -9981,7 +9981,7 @@
         <v>17898947389490</v>
       </c>
       <c r="E23" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
         <v>46</v>
@@ -10004,7 +10004,7 @@
         <v>17896075711930</v>
       </c>
       <c r="E24" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
         <v>64</v>
@@ -10027,7 +10027,7 @@
         <v>17896075710070</v>
       </c>
       <c r="E25" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
         <v>67</v>
@@ -10050,7 +10050,7 @@
         <v>17896075710100</v>
       </c>
       <c r="E26" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
         <v>70</v>
@@ -10073,7 +10073,7 @@
         <v>17896075711947</v>
       </c>
       <c r="E27" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s">
         <v>64</v>
@@ -10096,7 +10096,7 @@
         <v>17896540900845</v>
       </c>
       <c r="E28" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
         <v>75</v>
@@ -10119,7 +10119,7 @@
         <v>17896540900852</v>
       </c>
       <c r="E29" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
         <v>78</v>
@@ -10142,7 +10142,7 @@
         <v>17896540901774</v>
       </c>
       <c r="E30" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
         <v>81</v>
@@ -10165,7 +10165,7 @@
         <v>17896540901804</v>
       </c>
       <c r="E31" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
         <v>84</v>
@@ -10188,7 +10188,7 @@
         <v>17896540905215</v>
       </c>
       <c r="E32" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F32" t="s">
         <v>87</v>
@@ -10211,7 +10211,7 @@
         <v>17896540905208</v>
       </c>
       <c r="E33" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
         <v>87</v>
@@ -10234,7 +10234,7 @@
         <v>17896540905390</v>
       </c>
       <c r="E34" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F34" t="s">
         <v>92</v>
@@ -10257,7 +10257,7 @@
         <v>17896540905406</v>
       </c>
       <c r="E35" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F35" t="s">
         <v>95</v>
@@ -10280,7 +10280,7 @@
         <v>17896540905468</v>
       </c>
       <c r="E36" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F36" t="s">
         <v>98</v>
@@ -10303,7 +10303,7 @@
         <v>17896540905451</v>
       </c>
       <c r="E37" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
         <v>101</v>
@@ -10326,7 +10326,7 @@
         <v>17896540905444</v>
       </c>
       <c r="E38" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
         <v>101</v>
@@ -10349,7 +10349,7 @@
         <v>17896540905499</v>
       </c>
       <c r="E39" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
         <v>106</v>
@@ -10372,7 +10372,7 @@
         <v>17896540905628</v>
       </c>
       <c r="E40" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
         <v>109</v>
@@ -10395,7 +10395,7 @@
         <v>17896540905611</v>
       </c>
       <c r="E41" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
         <v>112</v>
@@ -10418,7 +10418,7 @@
         <v>57891040178075</v>
       </c>
       <c r="E42" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s">
         <v>115</v>
@@ -10441,7 +10441,7 @@
         <v>57891040177870</v>
       </c>
       <c r="E43" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
         <v>118</v>
@@ -10464,7 +10464,7 @@
         <v>57891040178068</v>
       </c>
       <c r="E44" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
         <v>115</v>
@@ -10487,7 +10487,7 @@
         <v>57891040177818</v>
       </c>
       <c r="E45" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F45" t="s">
         <v>115</v>
@@ -10510,7 +10510,7 @@
         <v>57891040178228</v>
       </c>
       <c r="E46" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F46" t="s">
         <v>115</v>
@@ -10533,7 +10533,7 @@
         <v>57891040178211</v>
       </c>
       <c r="E47" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F47" t="s">
         <v>115</v>
@@ -10556,7 +10556,7 @@
         <v>17896540901248</v>
       </c>
       <c r="E48" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F48" t="s">
         <v>129</v>
@@ -10579,7 +10579,7 @@
         <v>17896540901217</v>
       </c>
       <c r="E49" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F49" t="s">
         <v>129</v>
@@ -10602,7 +10602,7 @@
         <v>87896027093038</v>
       </c>
       <c r="E50" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F50" t="s">
         <v>134</v>
@@ -10625,7 +10625,7 @@
         <v>37896027093101</v>
       </c>
       <c r="E51" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
         <v>137</v>
@@ -10648,7 +10648,7 @@
         <v>17890310130463</v>
       </c>
       <c r="E52" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F52" t="s">
         <v>140</v>
@@ -10671,7 +10671,7 @@
         <v>17890310130456</v>
       </c>
       <c r="E53" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F53" t="s">
         <v>143</v>
@@ -10694,7 +10694,7 @@
         <v>17890310130845</v>
       </c>
       <c r="E54" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F54" t="s">
         <v>146</v>
@@ -10717,7 +10717,7 @@
         <v>17890310130449</v>
       </c>
       <c r="E55" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F55" t="s">
         <v>149</v>
@@ -10740,7 +10740,7 @@
         <v>17890310130487</v>
       </c>
       <c r="E56" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F56" t="s">
         <v>152</v>
@@ -10763,7 +10763,7 @@
         <v>17898185412202</v>
       </c>
       <c r="E57" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F57" t="s">
         <v>155</v>
@@ -10786,7 +10786,7 @@
         <v>17898185410512</v>
       </c>
       <c r="E58" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F58" t="s">
         <v>152</v>
@@ -10809,7 +10809,7 @@
         <v>17890310130814</v>
       </c>
       <c r="E59" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F59" t="s">
         <v>160</v>
@@ -10832,7 +10832,7 @@
         <v>17898185410499</v>
       </c>
       <c r="E60" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F60" t="s">
         <v>163</v>
@@ -10855,7 +10855,7 @@
         <v>17898624050545</v>
       </c>
       <c r="E61" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F61" t="s">
         <v>166</v>
@@ -10878,7 +10878,7 @@
         <v>17890310130593</v>
       </c>
       <c r="E62" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F62" t="s">
         <v>169</v>
@@ -10901,7 +10901,7 @@
         <v>17890310130807</v>
       </c>
       <c r="E63" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F63" t="s">
         <v>169</v>
@@ -10924,7 +10924,7 @@
         <v>17898624050552</v>
       </c>
       <c r="E64" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F64" t="s">
         <v>166</v>
@@ -10947,7 +10947,7 @@
         <v>17898185411113</v>
       </c>
       <c r="E65" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F65" t="s">
         <v>176</v>
@@ -10970,7 +10970,7 @@
         <v>17898185413230</v>
       </c>
       <c r="E66" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F66" t="s">
         <v>176</v>
@@ -10993,7 +10993,7 @@
         <v>17898949961076</v>
       </c>
       <c r="E67" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F67" t="s">
         <v>181</v>
@@ -11016,7 +11016,7 @@
         <v>7899706146258</v>
       </c>
       <c r="E68" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F68" t="s">
         <v>184</v>
@@ -11039,7 +11039,7 @@
         <v>7898587775236</v>
       </c>
       <c r="E69" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F69" t="s">
         <v>187</v>
@@ -11062,7 +11062,7 @@
         <v>7899706149587</v>
       </c>
       <c r="E70" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F70" t="s">
         <v>70</v>
@@ -11085,7 +11085,7 @@
         <v>7899706149624</v>
       </c>
       <c r="E71" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F71" t="s">
         <v>70</v>
@@ -11108,7 +11108,7 @@
         <v>7899026435124</v>
       </c>
       <c r="E72" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F72" t="s">
         <v>194</v>
@@ -11131,7 +11131,7 @@
         <v>7899026435162</v>
       </c>
       <c r="E73" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F73" t="s">
         <v>194</v>
@@ -11154,7 +11154,7 @@
         <v>7899706116534</v>
       </c>
       <c r="E74" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F74" t="s">
         <v>199</v>
@@ -11177,7 +11177,7 @@
         <v>7899706116541</v>
       </c>
       <c r="E75" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F75" t="s">
         <v>199</v>
@@ -11200,7 +11200,7 @@
         <v>7899706116565</v>
       </c>
       <c r="E76" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F76" t="s">
         <v>204</v>
@@ -11223,7 +11223,7 @@
         <v>7899706116572</v>
       </c>
       <c r="E77" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F77" t="s">
         <v>199</v>
@@ -11246,7 +11246,7 @@
         <v>7899706116589</v>
       </c>
       <c r="E78" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F78" t="s">
         <v>199</v>
@@ -11269,7 +11269,7 @@
         <v>7899706116619</v>
       </c>
       <c r="E79" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F79" t="s">
         <v>211</v>
@@ -11292,7 +11292,7 @@
         <v>7899706116626</v>
       </c>
       <c r="E80" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F80" t="s">
         <v>214</v>
@@ -11315,7 +11315,7 @@
         <v>7899706116640</v>
       </c>
       <c r="E81" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F81" t="s">
         <v>214</v>
@@ -11338,7 +11338,7 @@
         <v>7899706116657</v>
       </c>
       <c r="E82" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F82" t="s">
         <v>214</v>
@@ -11361,7 +11361,7 @@
         <v>7899706116664</v>
       </c>
       <c r="E83" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F83" t="s">
         <v>214</v>
@@ -11384,7 +11384,7 @@
         <v>7899706116749</v>
       </c>
       <c r="E84" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F84" t="s">
         <v>214</v>
@@ -11407,7 +11407,7 @@
         <v>7899706116756</v>
       </c>
       <c r="E85" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F85" t="s">
         <v>214</v>
@@ -11430,7 +11430,7 @@
         <v>7899706116763</v>
       </c>
       <c r="E86" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F86" t="s">
         <v>214</v>
@@ -11453,7 +11453,7 @@
         <v>7899706116770</v>
       </c>
       <c r="E87" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F87" t="s">
         <v>214</v>
@@ -11476,7 +11476,7 @@
         <v>7899706116787</v>
       </c>
       <c r="E88" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F88" t="s">
         <v>194</v>
@@ -11499,7 +11499,7 @@
         <v>7899706116800</v>
       </c>
       <c r="E89" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F89" t="s">
         <v>194</v>
@@ -11522,7 +11522,7 @@
         <v>7899706116824</v>
       </c>
       <c r="E90" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F90" t="s">
         <v>194</v>
@@ -11545,7 +11545,7 @@
         <v>7899706142083</v>
       </c>
       <c r="E91" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F91" t="s">
         <v>237</v>
@@ -11568,7 +11568,7 @@
         <v>7899706151900</v>
       </c>
       <c r="E92" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F92" t="s">
         <v>237</v>
@@ -11591,7 +11591,7 @@
         <v>7899706151870</v>
       </c>
       <c r="E93" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F93" t="s">
         <v>237</v>
@@ -11614,7 +11614,7 @@
         <v>7899706151863</v>
       </c>
       <c r="E94" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F94" t="s">
         <v>244</v>
@@ -11637,7 +11637,7 @@
         <v>7899706151887</v>
       </c>
       <c r="E95" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F95" t="s">
         <v>244</v>
@@ -11660,7 +11660,7 @@
         <v>7899706151856</v>
       </c>
       <c r="E96" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F96" t="s">
         <v>244</v>
@@ -11683,7 +11683,7 @@
         <v>7899706142090</v>
       </c>
       <c r="E97" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F97" t="s">
         <v>237</v>
@@ -11706,7 +11706,7 @@
         <v>7899706151894</v>
       </c>
       <c r="E98" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F98" t="s">
         <v>244</v>
@@ -11729,7 +11729,7 @@
         <v>7899706142113</v>
       </c>
       <c r="E99" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F99" t="s">
         <v>237</v>
@@ -11752,7 +11752,7 @@
         <v>7899706142120</v>
       </c>
       <c r="E100" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F100" t="s">
         <v>237</v>
@@ -11775,7 +11775,7 @@
         <v>7899706142144</v>
       </c>
       <c r="E101" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F101" t="s">
         <v>237</v>
@@ -11798,7 +11798,7 @@
         <v>7899706145732</v>
       </c>
       <c r="E102" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F102" t="s">
         <v>237</v>
@@ -11821,7 +11821,7 @@
         <v>7899706145725</v>
       </c>
       <c r="E103" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F103" t="s">
         <v>237</v>
@@ -11844,7 +11844,7 @@
         <v>7899706146470</v>
       </c>
       <c r="E104" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F104" t="s">
         <v>265</v>
@@ -11867,7 +11867,7 @@
         <v>7899706128308</v>
       </c>
       <c r="E105" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F105" t="s">
         <v>214</v>
@@ -11890,7 +11890,7 @@
         <v>7899706117333</v>
       </c>
       <c r="E106" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F106" t="s">
         <v>214</v>
@@ -11913,7 +11913,7 @@
         <v>7899706117340</v>
       </c>
       <c r="E107" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F107" t="s">
         <v>214</v>
@@ -11936,7 +11936,7 @@
         <v>7899706128254</v>
       </c>
       <c r="E108" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F108" t="s">
         <v>199</v>
@@ -11959,7 +11959,7 @@
         <v>7899706117357</v>
       </c>
       <c r="E109" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F109" t="s">
         <v>276</v>
@@ -11982,7 +11982,7 @@
         <v>7899706117371</v>
       </c>
       <c r="E110" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F110" t="s">
         <v>276</v>
@@ -12005,7 +12005,7 @@
         <v>7899706117388</v>
       </c>
       <c r="E111" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F111" t="s">
         <v>276</v>
@@ -12028,7 +12028,7 @@
         <v>7899706117401</v>
       </c>
       <c r="E112" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F112" t="s">
         <v>214</v>
@@ -12051,7 +12051,7 @@
         <v>7899706128285</v>
       </c>
       <c r="E113" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F113" t="s">
         <v>214</v>
@@ -12074,7 +12074,7 @@
         <v>7899706117418</v>
       </c>
       <c r="E114" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F114" t="s">
         <v>194</v>
@@ -12097,7 +12097,7 @@
         <v>7899706128292</v>
       </c>
       <c r="E115" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F115" t="s">
         <v>194</v>
@@ -12120,7 +12120,7 @@
         <v>17891040216151</v>
       </c>
       <c r="E116" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F116" t="s">
         <v>291</v>
@@ -12143,7 +12143,7 @@
         <v>57891040144254</v>
       </c>
       <c r="E117" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F117" t="s">
         <v>294</v>
@@ -12166,7 +12166,7 @@
         <v>57891040144247</v>
       </c>
       <c r="E118" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F118" t="s">
         <v>294</v>
@@ -12189,7 +12189,7 @@
         <v>57891040144278</v>
       </c>
       <c r="E119" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F119" t="s">
         <v>294</v>
@@ -12212,7 +12212,7 @@
         <v>17891040242075</v>
       </c>
       <c r="E120" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F120" t="s">
         <v>291</v>
@@ -12235,7 +12235,7 @@
         <v>57891040090926</v>
       </c>
       <c r="E121" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F121" t="s">
         <v>294</v>
@@ -12258,7 +12258,7 @@
         <v>17891040216113</v>
       </c>
       <c r="E122" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F122" t="s">
         <v>294</v>
@@ -12281,7 +12281,7 @@
         <v>17891040216137</v>
       </c>
       <c r="E123" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F123" t="s">
         <v>307</v>
@@ -12304,7 +12304,7 @@
         <v>17891040216120</v>
       </c>
       <c r="E124" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F124" t="s">
         <v>307</v>
@@ -12327,7 +12327,7 @@
         <v>17891040216106</v>
       </c>
       <c r="E125" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F125" t="s">
         <v>307</v>
@@ -12350,7 +12350,7 @@
         <v>17891040216090</v>
       </c>
       <c r="E126" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F126" t="s">
         <v>307</v>
@@ -12373,7 +12373,7 @@
         <v>17891040216144</v>
       </c>
       <c r="E127" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F127" t="s">
         <v>307</v>
@@ -12396,7 +12396,7 @@
         <v>17891040242082</v>
       </c>
       <c r="E128" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F128" t="s">
         <v>318</v>
@@ -12419,7 +12419,7 @@
         <v>7899706131896</v>
       </c>
       <c r="E129" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F129" t="s">
         <v>321</v>
@@ -12442,7 +12442,7 @@
         <v>7899706131902</v>
       </c>
       <c r="E130" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F130" t="s">
         <v>321</v>
@@ -12465,7 +12465,7 @@
         <v>7899706131919</v>
       </c>
       <c r="E131" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F131" t="s">
         <v>321</v>
@@ -12488,7 +12488,7 @@
         <v>7899706131940</v>
       </c>
       <c r="E132" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F132" t="s">
         <v>328</v>
@@ -12511,7 +12511,7 @@
         <v>57891040124157</v>
       </c>
       <c r="E133" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F133" t="s">
         <v>331</v>
@@ -12534,7 +12534,7 @@
         <v>17896075711886</v>
       </c>
       <c r="E134" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F134" t="s">
         <v>334</v>
@@ -12557,7 +12557,7 @@
         <v>17896075711862</v>
       </c>
       <c r="E135" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F135" t="s">
         <v>337</v>
@@ -12580,7 +12580,7 @@
         <v>17896075711893</v>
       </c>
       <c r="E136" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F136" t="s">
         <v>340</v>
@@ -12603,7 +12603,7 @@
         <v>67891040115886</v>
       </c>
       <c r="E137" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F137" t="s">
         <v>343</v>
@@ -12626,7 +12626,7 @@
         <v>47891040000348</v>
       </c>
       <c r="E138" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F138" t="s">
         <v>318</v>
@@ -12649,7 +12649,7 @@
         <v>47891040000324</v>
       </c>
       <c r="E139" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F139" t="s">
         <v>318</v>
@@ -12672,7 +12672,7 @@
         <v>47891040003875</v>
       </c>
       <c r="E140" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F140" t="s">
         <v>118</v>
@@ -12695,7 +12695,7 @@
         <v>67891040004128</v>
       </c>
       <c r="E141" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F141" t="s">
         <v>118</v>
@@ -12718,7 +12718,7 @@
         <v>37891040004134</v>
       </c>
       <c r="E142" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F142" t="s">
         <v>118</v>
@@ -12741,7 +12741,7 @@
         <v>17896509903528</v>
       </c>
       <c r="E143" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F143" t="s">
         <v>356</v>
@@ -12764,7 +12764,7 @@
         <v>17896509932139</v>
       </c>
       <c r="E144" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F144" t="s">
         <v>359</v>
@@ -12787,7 +12787,7 @@
         <v>17896509903566</v>
       </c>
       <c r="E145" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F145" t="s">
         <v>359</v>
@@ -12810,7 +12810,7 @@
         <v>17896509932146</v>
       </c>
       <c r="E146" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F146" t="s">
         <v>359</v>
@@ -12833,7 +12833,7 @@
         <v>17896509932153</v>
       </c>
       <c r="E147" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F147" t="s">
         <v>359</v>
@@ -12856,7 +12856,7 @@
         <v>17896509932160</v>
       </c>
       <c r="E148" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F148" t="s">
         <v>359</v>
@@ -12879,7 +12879,7 @@
         <v>17896509903047</v>
       </c>
       <c r="E149" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F149" t="s">
         <v>370</v>
@@ -12902,7 +12902,7 @@
         <v>17896509903054</v>
       </c>
       <c r="E150" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F150" t="s">
         <v>370</v>
@@ -12925,7 +12925,7 @@
         <v>17896509903061</v>
       </c>
       <c r="E151" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F151" t="s">
         <v>370</v>
@@ -12948,7 +12948,7 @@
         <v>17896509903078</v>
       </c>
       <c r="E152" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F152" t="s">
         <v>370</v>
@@ -12971,7 +12971,7 @@
         <v>17896509903085</v>
       </c>
       <c r="E153" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F153" t="s">
         <v>370</v>
@@ -12994,7 +12994,7 @@
         <v>17896509903092</v>
       </c>
       <c r="E154" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F154" t="s">
         <v>370</v>
@@ -13017,7 +13017,7 @@
         <v>17896509934812</v>
       </c>
       <c r="E155" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F155" t="s">
         <v>383</v>
@@ -13040,7 +13040,7 @@
         <v>17896509903115</v>
       </c>
       <c r="E156" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F156" t="s">
         <v>383</v>
@@ -13063,7 +13063,7 @@
         <v>17896509937424</v>
       </c>
       <c r="E157" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F157" t="s">
         <v>359</v>
@@ -13086,7 +13086,7 @@
         <v>17896509903122</v>
       </c>
       <c r="E158" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F158" t="s">
         <v>383</v>
@@ -13109,7 +13109,7 @@
         <v>17896509903153</v>
       </c>
       <c r="E159" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F159" t="s">
         <v>383</v>
@@ -13132,7 +13132,7 @@
         <v>17896509903177</v>
       </c>
       <c r="E160" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F160" t="s">
         <v>383</v>
@@ -13155,7 +13155,7 @@
         <v>17896509903207</v>
       </c>
       <c r="E161" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F161" t="s">
         <v>396</v>
@@ -13178,7 +13178,7 @@
         <v>17896509903214</v>
       </c>
       <c r="E162" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F162" t="s">
         <v>399</v>
@@ -13201,7 +13201,7 @@
         <v>17896509903221</v>
       </c>
       <c r="E163" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F163" t="s">
         <v>396</v>
@@ -13224,7 +13224,7 @@
         <v>17896509903238</v>
       </c>
       <c r="E164" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F164" t="s">
         <v>396</v>
@@ -13247,7 +13247,7 @@
         <v>17896509903252</v>
       </c>
       <c r="E165" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F165" t="s">
         <v>396</v>
@@ -13270,7 +13270,7 @@
         <v>17896509903269</v>
       </c>
       <c r="E166" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F166" t="s">
         <v>396</v>
@@ -13293,7 +13293,7 @@
         <v>17896509903306</v>
       </c>
       <c r="E167" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F167" t="s">
         <v>410</v>
@@ -13316,7 +13316,7 @@
         <v>17896509903313</v>
       </c>
       <c r="E168" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F168" t="s">
         <v>410</v>
@@ -13339,7 +13339,7 @@
         <v>17896509937974</v>
       </c>
       <c r="E169" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F169" t="s">
         <v>410</v>
@@ -13362,7 +13362,7 @@
         <v>17896509936373</v>
       </c>
       <c r="E170" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F170" t="s">
         <v>399</v>
@@ -13385,7 +13385,7 @@
         <v>17896509903320</v>
       </c>
       <c r="E171" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F171" t="s">
         <v>399</v>
@@ -13408,7 +13408,7 @@
         <v>17896509903337</v>
       </c>
       <c r="E172" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F172" t="s">
         <v>410</v>
@@ -13431,7 +13431,7 @@
         <v>17896509903344</v>
       </c>
       <c r="E173" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F173" t="s">
         <v>410</v>
@@ -13454,7 +13454,7 @@
         <v>17896509935062</v>
       </c>
       <c r="E174" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F174" t="s">
         <v>410</v>
@@ -13477,7 +13477,7 @@
         <v>17896509936380</v>
       </c>
       <c r="E175" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F175" t="s">
         <v>399</v>
@@ -13500,7 +13500,7 @@
         <v>17896509903429</v>
       </c>
       <c r="E176" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F176" t="s">
         <v>399</v>
@@ -13523,7 +13523,7 @@
         <v>17896509903436</v>
       </c>
       <c r="E177" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F177" t="s">
         <v>15</v>
@@ -13546,7 +13546,7 @@
         <v>17896509903443</v>
       </c>
       <c r="E178" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F178" t="s">
         <v>15</v>
@@ -13569,7 +13569,7 @@
         <v>17896509935123</v>
       </c>
       <c r="E179" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F179" t="s">
         <v>356</v>
@@ -13592,7 +13592,7 @@
         <v>17896509903481</v>
       </c>
       <c r="E180" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F180" t="s">
         <v>356</v>
@@ -13615,7 +13615,7 @@
         <v>17896509937431</v>
       </c>
       <c r="E181" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F181" t="s">
         <v>399</v>
@@ -13638,7 +13638,7 @@
         <v>17896509937929</v>
       </c>
       <c r="E182" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F182" t="s">
         <v>441</v>
@@ -13661,7 +13661,7 @@
         <v>7899706143011</v>
       </c>
       <c r="E183" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F183" t="s">
         <v>444</v>
@@ -13684,7 +13684,7 @@
         <v>17896014140432</v>
       </c>
       <c r="E184" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F184" t="s">
         <v>447</v>
@@ -13707,7 +13707,7 @@
         <v>17896014125248</v>
       </c>
       <c r="E185" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F185" t="s">
         <v>450</v>
@@ -13730,7 +13730,7 @@
         <v>17896014140692</v>
       </c>
       <c r="E186" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F186" t="s">
         <v>453</v>
@@ -13753,7 +13753,7 @@
         <v>17896509902989</v>
       </c>
       <c r="E187" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F187" t="s">
         <v>456</v>
@@ -13776,7 +13776,7 @@
         <v>17896014125422</v>
       </c>
       <c r="E188" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F188" t="s">
         <v>459</v>
@@ -13799,7 +13799,7 @@
         <v>17896014140708</v>
       </c>
       <c r="E189" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F189" t="s">
         <v>453</v>
@@ -13822,7 +13822,7 @@
         <v>17896509902996</v>
       </c>
       <c r="E190" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F190" t="s">
         <v>464</v>
@@ -13845,7 +13845,7 @@
         <v>17896509932108</v>
       </c>
       <c r="E191" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F191" t="s">
         <v>464</v>
@@ -13868,7 +13868,7 @@
         <v>17896509903023</v>
       </c>
       <c r="E192" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F192" t="s">
         <v>464</v>

</xml_diff>